<commit_message>
remove doenload link from hide code
</commit_message>
<xml_diff>
--- a/docs/memorias coletivas base dados.xlsx
+++ b/docs/memorias coletivas base dados.xlsx
@@ -6817,7 +6817,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P381" totalsRowShown="0">
-  <autoFilter ref="A1:P381"/>
+  <autoFilter ref="A1:P381">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="1941"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="16">
     <tableColumn id="1" name="filename"/>
     <tableColumn id="2" name="proprietario"/>
@@ -7130,10 +7136,10 @@
   <dimension ref="A1:P381"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P28" sqref="P28"/>
+      <selection pane="bottomRight" activeCell="E199" sqref="E199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7199,7 +7205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>377</v>
       </c>
@@ -7249,7 +7255,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>378</v>
       </c>
@@ -7299,7 +7305,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>379</v>
       </c>
@@ -7349,7 +7355,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>380</v>
       </c>
@@ -7399,7 +7405,7 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>381</v>
       </c>
@@ -7449,7 +7455,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>382</v>
       </c>
@@ -7499,7 +7505,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>383</v>
       </c>
@@ -7549,7 +7555,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>384</v>
       </c>
@@ -7599,7 +7605,7 @@
         <v>1862</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>385</v>
       </c>
@@ -7649,7 +7655,7 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>386</v>
       </c>
@@ -7699,7 +7705,7 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>387</v>
       </c>
@@ -7749,7 +7755,7 @@
         <v>1862</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>301</v>
       </c>
@@ -7799,7 +7805,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>302</v>
       </c>
@@ -7849,7 +7855,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>303</v>
       </c>
@@ -7899,7 +7905,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>304</v>
       </c>
@@ -7949,7 +7955,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>305</v>
       </c>
@@ -7999,7 +8005,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>306</v>
       </c>
@@ -8049,7 +8055,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>307</v>
       </c>
@@ -8099,7 +8105,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>308</v>
       </c>
@@ -8149,7 +8155,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>309</v>
       </c>
@@ -8199,7 +8205,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>310</v>
       </c>
@@ -8249,7 +8255,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>311</v>
       </c>
@@ -8299,7 +8305,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>312</v>
       </c>
@@ -8349,7 +8355,7 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>313</v>
       </c>
@@ -8399,7 +8405,7 @@
         <v>2042</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>314</v>
       </c>
@@ -8449,7 +8455,7 @@
         <v>1864</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>315</v>
       </c>
@@ -8499,7 +8505,7 @@
         <v>1865</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>316</v>
       </c>
@@ -8549,7 +8555,7 @@
         <v>1866</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>317</v>
       </c>
@@ -8599,7 +8605,7 @@
         <v>2042</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>318</v>
       </c>
@@ -8649,7 +8655,7 @@
         <v>2042</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>319</v>
       </c>
@@ -8699,7 +8705,7 @@
         <v>2042</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>320</v>
       </c>
@@ -8749,7 +8755,7 @@
         <v>2043</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>321</v>
       </c>
@@ -8799,7 +8805,7 @@
         <v>2111</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>322</v>
       </c>
@@ -8849,7 +8855,7 @@
         <v>2109</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>323</v>
       </c>
@@ -8899,7 +8905,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>324</v>
       </c>
@@ -8949,7 +8955,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>325</v>
       </c>
@@ -8999,7 +9005,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>326</v>
       </c>
@@ -9049,7 +9055,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>327</v>
       </c>
@@ -9099,7 +9105,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>328</v>
       </c>
@@ -9149,7 +9155,7 @@
         <v>2112</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>329</v>
       </c>
@@ -9199,7 +9205,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>330</v>
       </c>
@@ -9249,7 +9255,7 @@
         <v>2108</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>331</v>
       </c>
@@ -9299,7 +9305,7 @@
         <v>2109</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>332</v>
       </c>
@@ -9349,7 +9355,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>333</v>
       </c>
@@ -9399,7 +9405,7 @@
         <v>2044</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>334</v>
       </c>
@@ -9449,7 +9455,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>335</v>
       </c>
@@ -9499,7 +9505,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>336</v>
       </c>
@@ -9549,7 +9555,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>337</v>
       </c>
@@ -9599,7 +9605,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>338</v>
       </c>
@@ -9649,7 +9655,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>339</v>
       </c>
@@ -9699,7 +9705,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>340</v>
       </c>
@@ -9749,7 +9755,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>341</v>
       </c>
@@ -9799,7 +9805,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>342</v>
       </c>
@@ -9849,7 +9855,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>343</v>
       </c>
@@ -9899,7 +9905,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>344</v>
       </c>
@@ -9949,7 +9955,7 @@
         <v>1870</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>345</v>
       </c>
@@ -9999,7 +10005,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>346</v>
       </c>
@@ -10049,7 +10055,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>347</v>
       </c>
@@ -10099,7 +10105,7 @@
         <v>2042</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>348</v>
       </c>
@@ -10149,7 +10155,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>349</v>
       </c>
@@ -10199,7 +10205,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>350</v>
       </c>
@@ -10249,7 +10255,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>351</v>
       </c>
@@ -10299,7 +10305,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>352</v>
       </c>
@@ -10349,7 +10355,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>353</v>
       </c>
@@ -10399,7 +10405,7 @@
         <v>1871</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>354</v>
       </c>
@@ -10449,7 +10455,7 @@
         <v>1872</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>355</v>
       </c>
@@ -10499,7 +10505,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>356</v>
       </c>
@@ -10549,7 +10555,7 @@
         <v>2063</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>357</v>
       </c>
@@ -10599,7 +10605,7 @@
         <v>2063</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>358</v>
       </c>
@@ -10649,7 +10655,7 @@
         <v>2064</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>359</v>
       </c>
@@ -10699,7 +10705,7 @@
         <v>2063</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>360</v>
       </c>
@@ -10749,7 +10755,7 @@
         <v>2063</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>361</v>
       </c>
@@ -10799,7 +10805,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>362</v>
       </c>
@@ -10849,7 +10855,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>363</v>
       </c>
@@ -10899,7 +10905,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>364</v>
       </c>
@@ -10949,7 +10955,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>365</v>
       </c>
@@ -10999,7 +11005,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>366</v>
       </c>
@@ -11049,7 +11055,7 @@
         <v>1870</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>367</v>
       </c>
@@ -11099,7 +11105,7 @@
         <v>2066</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>368</v>
       </c>
@@ -11149,7 +11155,7 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>5</v>
       </c>
@@ -11199,7 +11205,7 @@
         <v>2171</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>369</v>
       </c>
@@ -11249,7 +11255,7 @@
         <v>2113</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>370</v>
       </c>
@@ -11299,7 +11305,7 @@
         <v>2114</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>371</v>
       </c>
@@ -11349,7 +11355,7 @@
         <v>2046</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>372</v>
       </c>
@@ -11399,7 +11405,7 @@
         <v>2055</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>373</v>
       </c>
@@ -11449,7 +11455,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>374</v>
       </c>
@@ -11499,7 +11505,7 @@
         <v>2042</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>375</v>
       </c>
@@ -11549,7 +11555,7 @@
         <v>1870</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>376</v>
       </c>
@@ -11599,7 +11605,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -11649,7 +11655,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>7</v>
       </c>
@@ -11699,7 +11705,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -11749,7 +11755,7 @@
         <v>2068</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>9</v>
       </c>
@@ -11799,7 +11805,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>10</v>
       </c>
@@ -11849,7 +11855,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>11</v>
       </c>
@@ -11899,7 +11905,7 @@
         <v>2116</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>12</v>
       </c>
@@ -11949,7 +11955,7 @@
         <v>2117</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>13</v>
       </c>
@@ -11999,7 +12005,7 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>14</v>
       </c>
@@ -12049,7 +12055,7 @@
         <v>2086</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>15</v>
       </c>
@@ -12099,7 +12105,7 @@
         <v>2069</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -12149,7 +12155,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>17</v>
       </c>
@@ -12199,7 +12205,7 @@
         <v>1874</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>18</v>
       </c>
@@ -12249,7 +12255,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="103" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>20</v>
       </c>
@@ -12299,7 +12305,7 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>21</v>
       </c>
@@ -12349,7 +12355,7 @@
         <v>2033</v>
       </c>
     </row>
-    <row r="105" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>22</v>
       </c>
@@ -12399,7 +12405,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="106" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>388</v>
       </c>
@@ -12443,7 +12449,7 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>389</v>
       </c>
@@ -12487,7 +12493,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="108" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>390</v>
       </c>
@@ -12531,7 +12537,7 @@
         <v>1877</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>391</v>
       </c>
@@ -12575,7 +12581,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="110" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>392</v>
       </c>
@@ -12619,7 +12625,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="111" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>393</v>
       </c>
@@ -12663,7 +12669,7 @@
         <v>1877</v>
       </c>
     </row>
-    <row r="112" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>394</v>
       </c>
@@ -12707,7 +12713,7 @@
         <v>2057</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>395</v>
       </c>
@@ -12751,7 +12757,7 @@
         <v>1879</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>396</v>
       </c>
@@ -12795,7 +12801,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>397</v>
       </c>
@@ -12839,7 +12845,7 @@
         <v>2035</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>398</v>
       </c>
@@ -12883,7 +12889,7 @@
         <v>2071</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>399</v>
       </c>
@@ -12927,7 +12933,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>400</v>
       </c>
@@ -12971,7 +12977,7 @@
         <v>2115</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>401</v>
       </c>
@@ -13015,7 +13021,7 @@
         <v>2072</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>402</v>
       </c>
@@ -13059,7 +13065,7 @@
         <v>1882</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>403</v>
       </c>
@@ -13103,7 +13109,7 @@
         <v>2178</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>404</v>
       </c>
@@ -13147,7 +13153,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>405</v>
       </c>
@@ -13191,7 +13197,7 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>406</v>
       </c>
@@ -13235,7 +13241,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="125" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>407</v>
       </c>
@@ -13279,7 +13285,7 @@
         <v>2073</v>
       </c>
     </row>
-    <row r="126" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>408</v>
       </c>
@@ -13323,7 +13329,7 @@
         <v>1884</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>409</v>
       </c>
@@ -13367,7 +13373,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="128" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>410</v>
       </c>
@@ -13411,7 +13417,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>411</v>
       </c>
@@ -13455,7 +13461,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="130" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>412</v>
       </c>
@@ -13499,7 +13505,7 @@
         <v>2031</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>413</v>
       </c>
@@ -13543,7 +13549,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>414</v>
       </c>
@@ -13587,7 +13593,7 @@
         <v>2088</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>415</v>
       </c>
@@ -13631,7 +13637,7 @@
         <v>2031</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>416</v>
       </c>
@@ -13675,7 +13681,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="135" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>417</v>
       </c>
@@ -13719,7 +13725,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="136" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>418</v>
       </c>
@@ -13763,7 +13769,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="137" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>419</v>
       </c>
@@ -13807,7 +13813,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="138" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>420</v>
       </c>
@@ -13851,7 +13857,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>421</v>
       </c>
@@ -13895,7 +13901,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>422</v>
       </c>
@@ -13939,7 +13945,7 @@
         <v>2107</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>423</v>
       </c>
@@ -13983,7 +13989,7 @@
         <v>2089</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>424</v>
       </c>
@@ -14027,7 +14033,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>425</v>
       </c>
@@ -14071,7 +14077,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>426</v>
       </c>
@@ -14115,7 +14121,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="145" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>427</v>
       </c>
@@ -14159,7 +14165,7 @@
         <v>2059</v>
       </c>
     </row>
-    <row r="146" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>428</v>
       </c>
@@ -14203,7 +14209,7 @@
         <v>2152</v>
       </c>
     </row>
-    <row r="147" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>429</v>
       </c>
@@ -14247,7 +14253,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="148" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>430</v>
       </c>
@@ -14291,7 +14297,7 @@
         <v>2130</v>
       </c>
     </row>
-    <row r="149" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>431</v>
       </c>
@@ -14335,7 +14341,7 @@
         <v>2093</v>
       </c>
     </row>
-    <row r="150" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>432</v>
       </c>
@@ -14379,7 +14385,7 @@
         <v>2094</v>
       </c>
     </row>
-    <row r="151" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>433</v>
       </c>
@@ -14423,7 +14429,7 @@
         <v>2095</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>434</v>
       </c>
@@ -14467,7 +14473,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="153" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>435</v>
       </c>
@@ -14511,7 +14517,7 @@
         <v>2096</v>
       </c>
     </row>
-    <row r="154" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>436</v>
       </c>
@@ -14555,7 +14561,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="155" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>437</v>
       </c>
@@ -14599,7 +14605,7 @@
         <v>2131</v>
       </c>
     </row>
-    <row r="156" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>438</v>
       </c>
@@ -14643,7 +14649,7 @@
         <v>1895</v>
       </c>
     </row>
-    <row r="157" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>439</v>
       </c>
@@ -14687,7 +14693,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="158" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>440</v>
       </c>
@@ -14731,7 +14737,7 @@
         <v>2097</v>
       </c>
     </row>
-    <row r="159" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>441</v>
       </c>
@@ -14775,7 +14781,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="160" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>442</v>
       </c>
@@ -14819,7 +14825,7 @@
         <v>2132</v>
       </c>
     </row>
-    <row r="161" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>443</v>
       </c>
@@ -14863,7 +14869,7 @@
         <v>1897</v>
       </c>
     </row>
-    <row r="162" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>444</v>
       </c>
@@ -14907,7 +14913,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="163" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>445</v>
       </c>
@@ -14951,7 +14957,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="164" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>446</v>
       </c>
@@ -14995,7 +15001,7 @@
         <v>1899</v>
       </c>
     </row>
-    <row r="165" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>447</v>
       </c>
@@ -15039,7 +15045,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="166" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>448</v>
       </c>
@@ -15083,7 +15089,7 @@
         <v>1901</v>
       </c>
     </row>
-    <row r="167" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>449</v>
       </c>
@@ -15127,7 +15133,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="168" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>450</v>
       </c>
@@ -15171,7 +15177,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="169" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>451</v>
       </c>
@@ -15215,7 +15221,7 @@
         <v>1903</v>
       </c>
     </row>
-    <row r="170" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>452</v>
       </c>
@@ -15259,7 +15265,7 @@
         <v>2091</v>
       </c>
     </row>
-    <row r="171" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>453</v>
       </c>
@@ -15303,7 +15309,7 @@
         <v>2076</v>
       </c>
     </row>
-    <row r="172" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>454</v>
       </c>
@@ -15347,7 +15353,7 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="173" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>455</v>
       </c>
@@ -15391,7 +15397,7 @@
         <v>2077</v>
       </c>
     </row>
-    <row r="174" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>456</v>
       </c>
@@ -15435,7 +15441,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="175" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>457</v>
       </c>
@@ -15479,7 +15485,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="176" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>458</v>
       </c>
@@ -15523,7 +15529,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="177" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>459</v>
       </c>
@@ -15567,7 +15573,7 @@
         <v>1906</v>
       </c>
     </row>
-    <row r="178" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>460</v>
       </c>
@@ -15611,7 +15617,7 @@
         <v>1907</v>
       </c>
     </row>
-    <row r="179" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>461</v>
       </c>
@@ -15655,7 +15661,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="180" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>462</v>
       </c>
@@ -15699,7 +15705,7 @@
         <v>2099</v>
       </c>
     </row>
-    <row r="181" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>463</v>
       </c>
@@ -15743,7 +15749,7 @@
         <v>2169</v>
       </c>
     </row>
-    <row r="182" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>464</v>
       </c>
@@ -15787,7 +15793,7 @@
         <v>1909</v>
       </c>
     </row>
-    <row r="183" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>465</v>
       </c>
@@ -15831,7 +15837,7 @@
         <v>1910</v>
       </c>
     </row>
-    <row r="184" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>466</v>
       </c>
@@ -15875,7 +15881,7 @@
         <v>2092</v>
       </c>
     </row>
-    <row r="185" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>467</v>
       </c>
@@ -15919,7 +15925,7 @@
         <v>2078</v>
       </c>
     </row>
-    <row r="186" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>468</v>
       </c>
@@ -15963,7 +15969,7 @@
         <v>1911</v>
       </c>
     </row>
-    <row r="187" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>469</v>
       </c>
@@ -16007,7 +16013,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="188" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>470</v>
       </c>
@@ -16051,7 +16057,7 @@
         <v>1912</v>
       </c>
     </row>
-    <row r="189" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>471</v>
       </c>
@@ -16095,7 +16101,7 @@
         <v>1913</v>
       </c>
     </row>
-    <row r="190" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>472</v>
       </c>
@@ -16139,7 +16145,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="191" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>473</v>
       </c>
@@ -16183,7 +16189,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="192" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>474</v>
       </c>
@@ -16227,7 +16233,7 @@
         <v>2133</v>
       </c>
     </row>
-    <row r="193" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>475</v>
       </c>
@@ -16271,7 +16277,7 @@
         <v>2078</v>
       </c>
     </row>
-    <row r="194" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>476</v>
       </c>
@@ -16315,7 +16321,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="195" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>477</v>
       </c>
@@ -16365,7 +16371,7 @@
         <v>1916</v>
       </c>
     </row>
-    <row r="196" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>478</v>
       </c>
@@ -16415,7 +16421,7 @@
         <v>2185</v>
       </c>
     </row>
-    <row r="197" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>479</v>
       </c>
@@ -16465,7 +16471,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="198" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>480</v>
       </c>
@@ -16523,7 +16529,7 @@
         <v>1785</v>
       </c>
       <c r="E199" s="6">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="F199" s="15">
         <v>1941</v>
@@ -16559,7 +16565,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="200" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>482</v>
       </c>
@@ -16603,7 +16609,7 @@
         <v>1918</v>
       </c>
     </row>
-    <row r="201" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>483</v>
       </c>
@@ -16647,7 +16653,7 @@
         <v>1919</v>
       </c>
     </row>
-    <row r="202" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>484</v>
       </c>
@@ -16691,7 +16697,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="203" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>485</v>
       </c>
@@ -16735,7 +16741,7 @@
         <v>1921</v>
       </c>
     </row>
-    <row r="204" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>486</v>
       </c>
@@ -16779,7 +16785,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="205" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>487</v>
       </c>
@@ -16823,7 +16829,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="206" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>488</v>
       </c>
@@ -16867,7 +16873,7 @@
         <v>1923</v>
       </c>
     </row>
-    <row r="207" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>489</v>
       </c>
@@ -16911,7 +16917,7 @@
         <v>1924</v>
       </c>
     </row>
-    <row r="208" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>490</v>
       </c>
@@ -16955,7 +16961,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="209" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>491</v>
       </c>
@@ -16999,7 +17005,7 @@
         <v>1926</v>
       </c>
     </row>
-    <row r="210" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>492</v>
       </c>
@@ -17043,7 +17049,7 @@
         <v>2168</v>
       </c>
     </row>
-    <row r="211" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>493</v>
       </c>
@@ -17087,7 +17093,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="212" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>494</v>
       </c>
@@ -17131,7 +17137,7 @@
         <v>1927</v>
       </c>
     </row>
-    <row r="213" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>495</v>
       </c>
@@ -17175,7 +17181,7 @@
         <v>1928</v>
       </c>
     </row>
-    <row r="214" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>496</v>
       </c>
@@ -17219,7 +17225,7 @@
         <v>1929</v>
       </c>
     </row>
-    <row r="215" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>497</v>
       </c>
@@ -17263,7 +17269,7 @@
         <v>1930</v>
       </c>
     </row>
-    <row r="216" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>498</v>
       </c>
@@ -17307,7 +17313,7 @@
         <v>1930</v>
       </c>
     </row>
-    <row r="217" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>499</v>
       </c>
@@ -17351,7 +17357,7 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="218" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>500</v>
       </c>
@@ -17395,7 +17401,7 @@
         <v>1931</v>
       </c>
     </row>
-    <row r="219" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>501</v>
       </c>
@@ -17439,7 +17445,7 @@
         <v>1932</v>
       </c>
     </row>
-    <row r="220" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>502</v>
       </c>
@@ -17483,7 +17489,7 @@
         <v>2101</v>
       </c>
     </row>
-    <row r="221" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>503</v>
       </c>
@@ -17527,7 +17533,7 @@
         <v>1882</v>
       </c>
     </row>
-    <row r="222" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>504</v>
       </c>
@@ -17571,7 +17577,7 @@
         <v>1933</v>
       </c>
     </row>
-    <row r="223" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>505</v>
       </c>
@@ -17615,7 +17621,7 @@
         <v>1934</v>
       </c>
     </row>
-    <row r="224" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>506</v>
       </c>
@@ -17659,7 +17665,7 @@
         <v>2134</v>
       </c>
     </row>
-    <row r="225" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>507</v>
       </c>
@@ -17703,7 +17709,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="226" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>508</v>
       </c>
@@ -17747,7 +17753,7 @@
         <v>2056</v>
       </c>
     </row>
-    <row r="227" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>509</v>
       </c>
@@ -17791,7 +17797,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="228" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>510</v>
       </c>
@@ -17835,7 +17841,7 @@
         <v>1935</v>
       </c>
     </row>
-    <row r="229" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>511</v>
       </c>
@@ -17879,7 +17885,7 @@
         <v>1936</v>
       </c>
     </row>
-    <row r="230" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>512</v>
       </c>
@@ -17923,7 +17929,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="231" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>513</v>
       </c>
@@ -17973,7 +17979,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="232" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>514</v>
       </c>
@@ -18023,7 +18029,7 @@
         <v>1937</v>
       </c>
     </row>
-    <row r="233" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>515</v>
       </c>
@@ -18073,7 +18079,7 @@
         <v>1938</v>
       </c>
     </row>
-    <row r="234" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>516</v>
       </c>
@@ -18123,7 +18129,7 @@
         <v>1939</v>
       </c>
     </row>
-    <row r="235" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>517</v>
       </c>
@@ -18173,7 +18179,7 @@
         <v>1940</v>
       </c>
     </row>
-    <row r="236" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>518</v>
       </c>
@@ -18223,7 +18229,7 @@
         <v>1941</v>
       </c>
     </row>
-    <row r="237" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>519</v>
       </c>
@@ -18273,7 +18279,7 @@
         <v>1942</v>
       </c>
     </row>
-    <row r="238" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>520</v>
       </c>
@@ -18323,7 +18329,7 @@
         <v>1943</v>
       </c>
     </row>
-    <row r="239" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>521</v>
       </c>
@@ -18367,7 +18373,7 @@
         <v>2137</v>
       </c>
     </row>
-    <row r="240" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>522</v>
       </c>
@@ -18417,7 +18423,7 @@
         <v>1944</v>
       </c>
     </row>
-    <row r="241" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>523</v>
       </c>
@@ -18461,7 +18467,7 @@
         <v>1945</v>
       </c>
     </row>
-    <row r="242" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>524</v>
       </c>
@@ -18505,7 +18511,7 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="243" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>525</v>
       </c>
@@ -18549,7 +18555,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="244" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>526</v>
       </c>
@@ -18599,7 +18605,7 @@
         <v>2138</v>
       </c>
     </row>
-    <row r="245" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>527</v>
       </c>
@@ -18643,7 +18649,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="246" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>528</v>
       </c>
@@ -18687,7 +18693,7 @@
         <v>2156</v>
       </c>
     </row>
-    <row r="247" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>529</v>
       </c>
@@ -18731,7 +18737,7 @@
         <v>2156</v>
       </c>
     </row>
-    <row r="248" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>530</v>
       </c>
@@ -18775,7 +18781,7 @@
         <v>2102</v>
       </c>
     </row>
-    <row r="249" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>531</v>
       </c>
@@ -18819,7 +18825,7 @@
         <v>1947</v>
       </c>
     </row>
-    <row r="250" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>532</v>
       </c>
@@ -18863,7 +18869,7 @@
         <v>2103</v>
       </c>
     </row>
-    <row r="251" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>533</v>
       </c>
@@ -18907,7 +18913,7 @@
         <v>1947</v>
       </c>
     </row>
-    <row r="252" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>534</v>
       </c>
@@ -18951,7 +18957,7 @@
         <v>1947</v>
       </c>
     </row>
-    <row r="253" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>535</v>
       </c>
@@ -18995,7 +19001,7 @@
         <v>1947</v>
       </c>
     </row>
-    <row r="254" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>536</v>
       </c>
@@ -19039,7 +19045,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="255" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>537</v>
       </c>
@@ -19083,7 +19089,7 @@
         <v>1948</v>
       </c>
     </row>
-    <row r="256" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>538</v>
       </c>
@@ -19133,7 +19139,7 @@
         <v>1949</v>
       </c>
     </row>
-    <row r="257" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>539</v>
       </c>
@@ -19183,7 +19189,7 @@
         <v>1949</v>
       </c>
     </row>
-    <row r="258" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>540</v>
       </c>
@@ -19227,7 +19233,7 @@
         <v>1949</v>
       </c>
     </row>
-    <row r="259" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>541</v>
       </c>
@@ -19277,7 +19283,7 @@
         <v>1949</v>
       </c>
     </row>
-    <row r="260" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>542</v>
       </c>
@@ -19321,7 +19327,7 @@
         <v>2081</v>
       </c>
     </row>
-    <row r="261" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>543</v>
       </c>
@@ -19371,7 +19377,7 @@
         <v>2180</v>
       </c>
     </row>
-    <row r="262" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>544</v>
       </c>
@@ -19421,7 +19427,7 @@
         <v>2181</v>
       </c>
     </row>
-    <row r="263" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>545</v>
       </c>
@@ -19465,7 +19471,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="264" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>546</v>
       </c>
@@ -19509,7 +19515,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="265" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>547</v>
       </c>
@@ -19553,7 +19559,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="266" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>548</v>
       </c>
@@ -19597,7 +19603,7 @@
         <v>2175</v>
       </c>
     </row>
-    <row r="267" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>549</v>
       </c>
@@ -19641,7 +19647,7 @@
         <v>2176</v>
       </c>
     </row>
-    <row r="268" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>550</v>
       </c>
@@ -19685,7 +19691,7 @@
         <v>2182</v>
       </c>
     </row>
-    <row r="269" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>551</v>
       </c>
@@ -19729,7 +19735,7 @@
         <v>2176</v>
       </c>
     </row>
-    <row r="270" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>552</v>
       </c>
@@ -19773,7 +19779,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="271" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>553</v>
       </c>
@@ -19817,7 +19823,7 @@
         <v>2123</v>
       </c>
     </row>
-    <row r="272" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>554</v>
       </c>
@@ -19861,7 +19867,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="273" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>555</v>
       </c>
@@ -19905,7 +19911,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="274" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>556</v>
       </c>
@@ -19949,7 +19955,7 @@
         <v>2167</v>
       </c>
     </row>
-    <row r="275" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>557</v>
       </c>
@@ -19993,7 +19999,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="276" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>558</v>
       </c>
@@ -20037,7 +20043,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="277" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>559</v>
       </c>
@@ -20087,7 +20093,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="278" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>560</v>
       </c>
@@ -20131,7 +20137,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="279" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>561</v>
       </c>
@@ -20181,7 +20187,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="280" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>562</v>
       </c>
@@ -20231,7 +20237,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="281" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>563</v>
       </c>
@@ -20275,7 +20281,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="282" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>564</v>
       </c>
@@ -20325,7 +20331,7 @@
         <v>2124</v>
       </c>
     </row>
-    <row r="283" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>565</v>
       </c>
@@ -20370,7 +20376,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="284" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>566</v>
       </c>
@@ -20414,7 +20420,7 @@
         <v>2126</v>
       </c>
     </row>
-    <row r="285" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>567</v>
       </c>
@@ -20464,7 +20470,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="286" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>568</v>
       </c>
@@ -20514,7 +20520,7 @@
         <v>1951</v>
       </c>
     </row>
-    <row r="287" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>569</v>
       </c>
@@ -20558,7 +20564,7 @@
         <v>1952</v>
       </c>
     </row>
-    <row r="288" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>570</v>
       </c>
@@ -20608,7 +20614,7 @@
         <v>1953</v>
       </c>
     </row>
-    <row r="289" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>571</v>
       </c>
@@ -20658,7 +20664,7 @@
         <v>1953</v>
       </c>
     </row>
-    <row r="290" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>572</v>
       </c>
@@ -20708,7 +20714,7 @@
         <v>1954</v>
       </c>
     </row>
-    <row r="291" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>573</v>
       </c>
@@ -20752,7 +20758,7 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="292" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>574</v>
       </c>
@@ -20796,7 +20802,7 @@
         <v>1955</v>
       </c>
     </row>
-    <row r="293" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>575</v>
       </c>
@@ -20840,7 +20846,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="294" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>576</v>
       </c>
@@ -20884,7 +20890,7 @@
         <v>1957</v>
       </c>
     </row>
-    <row r="295" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>577</v>
       </c>
@@ -20928,7 +20934,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="296" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>578</v>
       </c>
@@ -20972,7 +20978,7 @@
         <v>2186</v>
       </c>
     </row>
-    <row r="297" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>579</v>
       </c>
@@ -21016,7 +21022,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="298" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>580</v>
       </c>
@@ -21066,7 +21072,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="299" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>581</v>
       </c>
@@ -21116,7 +21122,7 @@
         <v>2157</v>
       </c>
     </row>
-    <row r="300" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>582</v>
       </c>
@@ -21166,7 +21172,7 @@
         <v>1961</v>
       </c>
     </row>
-    <row r="301" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>583</v>
       </c>
@@ -21216,7 +21222,7 @@
         <v>1962</v>
       </c>
     </row>
-    <row r="302" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>584</v>
       </c>
@@ -21266,7 +21272,7 @@
         <v>2139</v>
       </c>
     </row>
-    <row r="303" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>585</v>
       </c>
@@ -21316,7 +21322,7 @@
         <v>1963</v>
       </c>
     </row>
-    <row r="304" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>586</v>
       </c>
@@ -21366,7 +21372,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="305" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>587</v>
       </c>
@@ -21416,7 +21422,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="306" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>588</v>
       </c>
@@ -21466,7 +21472,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="307" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>589</v>
       </c>
@@ -21516,7 +21522,7 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="308" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>590</v>
       </c>
@@ -21560,7 +21566,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="309" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>591</v>
       </c>
@@ -21610,7 +21616,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="310" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>592</v>
       </c>
@@ -21660,7 +21666,7 @@
         <v>2158</v>
       </c>
     </row>
-    <row r="311" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>593</v>
       </c>
@@ -21710,7 +21716,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="312" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>594</v>
       </c>
@@ -21760,7 +21766,7 @@
         <v>2140</v>
       </c>
     </row>
-    <row r="313" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>595</v>
       </c>
@@ -21810,7 +21816,7 @@
         <v>2099</v>
       </c>
     </row>
-    <row r="314" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>596</v>
       </c>
@@ -21860,7 +21866,7 @@
         <v>2184</v>
       </c>
     </row>
-    <row r="315" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>597</v>
       </c>
@@ -21910,7 +21916,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="316" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>598</v>
       </c>
@@ -21960,7 +21966,7 @@
         <v>2105</v>
       </c>
     </row>
-    <row r="317" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>599</v>
       </c>
@@ -22010,7 +22016,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="318" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>600</v>
       </c>
@@ -22060,7 +22066,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="319" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>601</v>
       </c>
@@ -22104,7 +22110,7 @@
         <v>2141</v>
       </c>
     </row>
-    <row r="320" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>602</v>
       </c>
@@ -22154,7 +22160,7 @@
         <v>2142</v>
       </c>
     </row>
-    <row r="321" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>603</v>
       </c>
@@ -22198,7 +22204,7 @@
         <v>2149</v>
       </c>
     </row>
-    <row r="322" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>604</v>
       </c>
@@ -22242,7 +22248,7 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="323" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>605</v>
       </c>
@@ -22286,7 +22292,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="324" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>606</v>
       </c>
@@ -22330,7 +22336,7 @@
         <v>2162</v>
       </c>
     </row>
-    <row r="325" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>607</v>
       </c>
@@ -22380,7 +22386,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="326" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>608</v>
       </c>
@@ -22427,7 +22433,7 @@
         <v>2153</v>
       </c>
     </row>
-    <row r="327" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>609</v>
       </c>
@@ -22471,7 +22477,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="328" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>610</v>
       </c>
@@ -22515,7 +22521,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="329" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>611</v>
       </c>
@@ -22559,7 +22565,7 @@
         <v>2144</v>
       </c>
     </row>
-    <row r="330" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>612</v>
       </c>
@@ -22609,7 +22615,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="331" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>613</v>
       </c>
@@ -22653,7 +22659,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="332" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>614</v>
       </c>
@@ -22697,7 +22703,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="333" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>615</v>
       </c>
@@ -22741,7 +22747,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="334" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>616</v>
       </c>
@@ -22791,7 +22797,7 @@
         <v>1977</v>
       </c>
     </row>
-    <row r="335" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>617</v>
       </c>
@@ -22841,7 +22847,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="336" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>618</v>
       </c>
@@ -22885,7 +22891,7 @@
         <v>2082</v>
       </c>
     </row>
-    <row r="337" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>619</v>
       </c>
@@ -22929,7 +22935,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="338" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>620</v>
       </c>
@@ -22979,7 +22985,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="339" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>621</v>
       </c>
@@ -23029,7 +23035,7 @@
         <v>2083</v>
       </c>
     </row>
-    <row r="340" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>622</v>
       </c>
@@ -23079,7 +23085,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="341" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>623</v>
       </c>
@@ -23129,7 +23135,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="342" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>624</v>
       </c>
@@ -23179,7 +23185,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="343" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>625</v>
       </c>
@@ -23229,7 +23235,7 @@
         <v>1983</v>
       </c>
     </row>
-    <row r="344" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>626</v>
       </c>
@@ -23273,7 +23279,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="345" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>627</v>
       </c>
@@ -23317,7 +23323,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="346" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>628</v>
       </c>
@@ -23361,7 +23367,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="347" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>629</v>
       </c>
@@ -23411,7 +23417,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="348" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>630</v>
       </c>
@@ -23455,7 +23461,7 @@
         <v>2087</v>
       </c>
     </row>
-    <row r="349" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>631</v>
       </c>
@@ -23505,7 +23511,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="350" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>632</v>
       </c>
@@ -23555,7 +23561,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="351" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>633</v>
       </c>
@@ -23605,7 +23611,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="352" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>634</v>
       </c>
@@ -23655,7 +23661,7 @@
         <v>2084</v>
       </c>
     </row>
-    <row r="353" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>635</v>
       </c>
@@ -23705,7 +23711,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="354" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>636</v>
       </c>
@@ -23755,7 +23761,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="355" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>637</v>
       </c>
@@ -23805,7 +23811,7 @@
         <v>2129</v>
       </c>
     </row>
-    <row r="356" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>638</v>
       </c>
@@ -23855,7 +23861,7 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="357" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>639</v>
       </c>
@@ -23899,7 +23905,7 @@
         <v>2106</v>
       </c>
     </row>
-    <row r="358" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>640</v>
       </c>
@@ -23943,7 +23949,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="359" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>641</v>
       </c>
@@ -23987,7 +23993,7 @@
         <v>2039</v>
       </c>
     </row>
-    <row r="360" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>642</v>
       </c>
@@ -24031,7 +24037,7 @@
         <v>2061</v>
       </c>
     </row>
-    <row r="361" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>643</v>
       </c>
@@ -24075,7 +24081,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="362" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>644</v>
       </c>
@@ -24119,7 +24125,7 @@
         <v>2058</v>
       </c>
     </row>
-    <row r="363" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>645</v>
       </c>
@@ -24163,7 +24169,7 @@
         <v>2061</v>
       </c>
     </row>
-    <row r="364" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>646</v>
       </c>
@@ -24207,7 +24213,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="365" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>647</v>
       </c>
@@ -24251,7 +24257,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="366" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>648</v>
       </c>
@@ -24295,7 +24301,7 @@
         <v>2051</v>
       </c>
     </row>
-    <row r="367" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>649</v>
       </c>
@@ -24339,7 +24345,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="368" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>650</v>
       </c>
@@ -24383,7 +24389,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="369" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>651</v>
       </c>
@@ -24427,7 +24433,7 @@
         <v>2161</v>
       </c>
     </row>
-    <row r="370" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>652</v>
       </c>
@@ -24471,7 +24477,7 @@
         <v>2052</v>
       </c>
     </row>
-    <row r="371" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>653</v>
       </c>
@@ -24515,7 +24521,7 @@
         <v>2041</v>
       </c>
     </row>
-    <row r="372" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>654</v>
       </c>
@@ -24559,7 +24565,7 @@
         <v>2062</v>
       </c>
     </row>
-    <row r="373" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>655</v>
       </c>
@@ -24603,7 +24609,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="374" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>656</v>
       </c>
@@ -24647,7 +24653,7 @@
         <v>2053</v>
       </c>
     </row>
-    <row r="375" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>657</v>
       </c>
@@ -24697,7 +24703,7 @@
         <v>2032</v>
       </c>
     </row>
-    <row r="376" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A376" s="12" t="s">
         <v>2000</v>
       </c>
@@ -24729,7 +24735,7 @@
         <v>2148</v>
       </c>
     </row>
-    <row r="377" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A377" s="12" t="s">
         <v>2001</v>
       </c>
@@ -24761,7 +24767,7 @@
         <v>2147</v>
       </c>
     </row>
-    <row r="378" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A378" s="12" t="s">
         <v>2002</v>
       </c>
@@ -24793,7 +24799,7 @@
         <v>2146</v>
       </c>
     </row>
-    <row r="379" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A379" s="12" t="s">
         <v>2003</v>
       </c>
@@ -24825,7 +24831,7 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="380" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A380" s="12" t="s">
         <v>2004</v>
       </c>
@@ -24857,7 +24863,7 @@
         <v>1871</v>
       </c>
     </row>
-    <row r="381" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:16" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A381" s="12" t="s">
         <v>2005</v>
       </c>

</xml_diff>